<commit_message>
trim & concatenate video clips
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -828,6 +828,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -849,6 +850,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -933,13 +935,13 @@
   </sheetPr>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.96"/>
@@ -1443,9 +1445,9 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +2857,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Oldal &amp;P</oddFooter>

</xml_diff>